<commit_message>
add question 14/08 by hieudn
</commit_message>
<xml_diff>
--- a/QA/通訳サービス_QA表_VN.xlsx
+++ b/QA/通訳サービス_QA表_VN.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MixiComputer\Desktop\Thuan\PJ\Interpretting Service\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieudn\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239B4D90-D815-4EC9-A653-8C5F7E6C0A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DADD1509-012E-4080-9D16-B96D878A527F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QA表" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="62">
   <si>
     <t>No</t>
   </si>
@@ -236,6 +236,18 @@
   </si>
   <si>
     <t>Ngoài source code, testcase, trường hợp smartphone app thì hãy gửi cả app sau khi build (andoroid,ios) cho chúng tôi nhé!</t>
+  </si>
+  <si>
+    <t>Nguyen Dang Hieu</t>
+  </si>
+  <si>
+    <t>Mô tả nội dung hiển thị (công thức tính toán) của từng mục như số cuộc gọi đến, số cuộc gọi đã nhận, tỉ lệ cuộc gọi nhận, số ghế hoạt động ( trung bình theo tháng) … Cuộc gọi chờ số lượng thoát tương ứng với file data json nào, và tương ứng với field giữ liệu nào?</t>
+  </si>
+  <si>
+    <t>Chúng tôi đang thấy material-ui: 4.5.1 hình như ko đúng version, vì version này ko dùng dc TableContainer, mà trong code mấy file của bạn gửi lại có dùng dc TableContainer. hiện tại thấy version 4.9.1 thì dùng dc. Chúng tôi có thể sử dụng version 4.9.1 này được không?</t>
+  </si>
+  <si>
+    <t>Trong bảng operator có nút setting. Chúng tôi không biết phương thức hoạt động của nút setting đó, không biết các bạn có nhầm nút setting đó với nút search không? Vui lòng mô tả rõ ràng cách hoạt động của nút này</t>
   </si>
 </sst>
 </file>
@@ -548,6 +560,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -557,47 +605,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -914,13 +926,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:K17"/>
+  <dimension ref="A2:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="H5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,7 +1000,7 @@
       <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="34" t="s">
         <v>39</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -1003,13 +1015,13 @@
       <c r="G5" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="27" t="s">
+      <c r="H5" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="I5" s="28" t="s">
+      <c r="I5" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="J5" s="29">
+      <c r="J5" s="24">
         <v>45513</v>
       </c>
       <c r="K5" s="3"/>
@@ -1019,7 +1031,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="9"/>
-      <c r="C6" s="23"/>
+      <c r="C6" s="35"/>
       <c r="D6" s="7" t="s">
         <v>16</v>
       </c>
@@ -1032,13 +1044,13 @@
       <c r="G6" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="30" t="s">
+      <c r="H6" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="I6" s="31" t="s">
+      <c r="I6" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="J6" s="32">
+      <c r="J6" s="27">
         <v>45513</v>
       </c>
       <c r="K6" s="3"/>
@@ -1050,7 +1062,7 @@
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="34" t="s">
         <v>40</v>
       </c>
       <c r="D7" s="7" t="s">
@@ -1065,13 +1077,13 @@
       <c r="G7" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="30" t="s">
+      <c r="H7" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="31" t="s">
+      <c r="I7" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="J7" s="32">
+      <c r="J7" s="27">
         <v>45513</v>
       </c>
       <c r="K7" s="3"/>
@@ -1081,7 +1093,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="10"/>
-      <c r="C8" s="24"/>
+      <c r="C8" s="36"/>
       <c r="D8" s="7" t="s">
         <v>17</v>
       </c>
@@ -1094,13 +1106,13 @@
       <c r="G8" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="30" t="s">
+      <c r="H8" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="I8" s="31" t="s">
+      <c r="I8" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="J8" s="32">
+      <c r="J8" s="27">
         <v>45513</v>
       </c>
       <c r="K8" s="3"/>
@@ -1110,7 +1122,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="10"/>
-      <c r="C9" s="24"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="7" t="s">
         <v>18</v>
       </c>
@@ -1123,13 +1135,13 @@
       <c r="G9" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="30" t="s">
+      <c r="H9" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="I9" s="33" t="s">
+      <c r="I9" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="J9" s="32">
+      <c r="J9" s="27">
         <v>45513</v>
       </c>
       <c r="K9" s="3"/>
@@ -1139,7 +1151,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="10"/>
-      <c r="C10" s="23"/>
+      <c r="C10" s="35"/>
       <c r="D10" s="7" t="s">
         <v>19</v>
       </c>
@@ -1152,13 +1164,13 @@
       <c r="G10" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="38" t="s">
+      <c r="H10" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="I10" s="33" t="s">
+      <c r="I10" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="J10" s="32">
+      <c r="J10" s="27">
         <v>45513</v>
       </c>
       <c r="K10" s="3"/>
@@ -1168,7 +1180,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="10"/>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="34" t="s">
         <v>41</v>
       </c>
       <c r="D11" s="7" t="s">
@@ -1183,13 +1195,13 @@
       <c r="G11" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="34" t="s">
+      <c r="H11" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="I11" s="31" t="s">
+      <c r="I11" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="J11" s="32">
+      <c r="J11" s="27">
         <v>45513</v>
       </c>
       <c r="K11" s="3"/>
@@ -1199,7 +1211,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="9"/>
-      <c r="C12" s="23"/>
+      <c r="C12" s="35"/>
       <c r="D12" s="7" t="s">
         <v>21</v>
       </c>
@@ -1212,13 +1224,13 @@
       <c r="G12" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="34" t="s">
+      <c r="H12" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="I12" s="33" t="s">
+      <c r="I12" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="J12" s="32">
+      <c r="J12" s="27">
         <v>45513</v>
       </c>
       <c r="K12" s="3"/>
@@ -1230,7 +1242,7 @@
       <c r="B13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="34" t="s">
         <v>42</v>
       </c>
       <c r="D13" s="7" t="s">
@@ -1245,13 +1257,13 @@
       <c r="G13" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="30" t="s">
+      <c r="H13" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="I13" s="33" t="s">
+      <c r="I13" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="J13" s="32">
+      <c r="J13" s="27">
         <v>45513</v>
       </c>
       <c r="K13" s="3"/>
@@ -1261,7 +1273,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="9"/>
-      <c r="C14" s="23"/>
+      <c r="C14" s="35"/>
       <c r="D14" s="7" t="s">
         <v>22</v>
       </c>
@@ -1274,13 +1286,13 @@
       <c r="G14" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="H14" s="30" t="s">
+      <c r="H14" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="I14" s="31" t="s">
+      <c r="I14" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="J14" s="32">
+      <c r="J14" s="27">
         <v>45513</v>
       </c>
       <c r="K14" s="3"/>
@@ -1289,8 +1301,8 @@
       <c r="A15" s="3">
         <v>11</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="25" t="s">
+      <c r="B15" s="37"/>
+      <c r="C15" s="38" t="s">
         <v>43</v>
       </c>
       <c r="D15" s="7" t="s">
@@ -1305,13 +1317,13 @@
       <c r="G15" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="H15" s="30" t="s">
+      <c r="H15" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="I15" s="31" t="s">
+      <c r="I15" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="J15" s="32">
+      <c r="J15" s="27">
         <v>45513</v>
       </c>
       <c r="K15" s="3"/>
@@ -1320,8 +1332,8 @@
       <c r="A16" s="3">
         <v>12</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="26"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="38"/>
       <c r="D16" s="7" t="s">
         <v>23</v>
       </c>
@@ -1334,18 +1346,87 @@
       <c r="G16" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="I16" s="36" t="s">
+      <c r="I16" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J16" s="37">
+      <c r="J16" s="32">
         <v>45513</v>
       </c>
       <c r="K16" s="3"/>
     </row>
-    <row r="17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:11" ht="55.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>13</v>
+      </c>
+      <c r="B17" s="37"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="11">
+        <v>45518</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="H17" s="30"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="1:11" ht="42" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>15</v>
+      </c>
+      <c r="B18" s="37"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="11">
+        <v>45518</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H18" s="30"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="1:11" ht="42" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>16</v>
+      </c>
+      <c r="B19" s="37"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" s="11">
+        <v>45518</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H19" s="30"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C5:C6"/>

</xml_diff>

<commit_message>
adđ QA relate to IOS device error
</commit_message>
<xml_diff>
--- a/QA/通訳サービス_QA表_VN.xlsx
+++ b/QA/通訳サービス_QA表_VN.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieudn\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\zeus-tmp\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DADD1509-012E-4080-9D16-B96D878A527F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5A3CD2-B7AF-46DA-BBAD-94C76261369D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QA表" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="65">
   <si>
     <t>No</t>
   </si>
@@ -248,6 +248,57 @@
   </si>
   <si>
     <t>Trong bảng operator có nút setting. Chúng tôi không biết phương thức hoạt động của nút setting đó, không biết các bạn có nhầm nút setting đó với nút search không? Vui lòng mô tả rõ ràng cách hoạt động của nút này</t>
+  </si>
+  <si>
+    <t>Bui Viet Hoang</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Khi sử dụng webview với các app build bằng IOS, chúng tôi có kết nối được với camera và microphone rồi và có thể bấm gọi. Nhưng khi bên trang "https://example.likeness-online.com/host" bấm </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="MS PGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>promote all</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="MS PGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> thì bên app báo lỗi là "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="MS PGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>Unable to join the room</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="MS PGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>". Chúng tôi muốn biết là có những yêu cầu về thiết bị hoặc dữ liệu nào mà các bạn cho phép và không cho phép để có thể tham gia phòng. Hy vọng các bạn có thể check error log giúp chúng tôi vì đây là webview và phần thông báo lỗi này là từ trên website.
+Dưới dây là url hình ảnh minh họa: https://ibb.co/jgh2ph2</t>
+    </r>
+  </si>
+  <si>
+    <t>データの検証</t>
   </si>
 </sst>
 </file>
@@ -257,7 +308,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -328,6 +379,21 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="MS PGothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="MS PGothic"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -596,6 +662,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -604,12 +676,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -926,13 +992,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:K20"/>
+  <dimension ref="A2:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
       <pane xSplit="4" ySplit="4" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
+      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1000,7 +1066,7 @@
       <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="36" t="s">
         <v>39</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -1031,7 +1097,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="9"/>
-      <c r="C6" s="35"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="7" t="s">
         <v>16</v>
       </c>
@@ -1062,7 +1128,7 @@
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="36" t="s">
         <v>40</v>
       </c>
       <c r="D7" s="7" t="s">
@@ -1093,7 +1159,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="10"/>
-      <c r="C8" s="36"/>
+      <c r="C8" s="38"/>
       <c r="D8" s="7" t="s">
         <v>17</v>
       </c>
@@ -1122,7 +1188,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="10"/>
-      <c r="C9" s="36"/>
+      <c r="C9" s="38"/>
       <c r="D9" s="7" t="s">
         <v>18</v>
       </c>
@@ -1151,7 +1217,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="10"/>
-      <c r="C10" s="35"/>
+      <c r="C10" s="37"/>
       <c r="D10" s="7" t="s">
         <v>19</v>
       </c>
@@ -1180,7 +1246,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="10"/>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="36" t="s">
         <v>41</v>
       </c>
       <c r="D11" s="7" t="s">
@@ -1211,7 +1277,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="9"/>
-      <c r="C12" s="35"/>
+      <c r="C12" s="37"/>
       <c r="D12" s="7" t="s">
         <v>21</v>
       </c>
@@ -1242,7 +1308,7 @@
       <c r="B13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="36" t="s">
         <v>42</v>
       </c>
       <c r="D13" s="7" t="s">
@@ -1273,7 +1339,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="9"/>
-      <c r="C14" s="35"/>
+      <c r="C14" s="37"/>
       <c r="D14" s="7" t="s">
         <v>22</v>
       </c>
@@ -1301,8 +1367,8 @@
       <c r="A15" s="3">
         <v>11</v>
       </c>
-      <c r="B15" s="37"/>
-      <c r="C15" s="38" t="s">
+      <c r="B15" s="34"/>
+      <c r="C15" s="35" t="s">
         <v>43</v>
       </c>
       <c r="D15" s="7" t="s">
@@ -1332,8 +1398,8 @@
       <c r="A16" s="3">
         <v>12</v>
       </c>
-      <c r="B16" s="37"/>
-      <c r="C16" s="38"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="35"/>
       <c r="D16" s="7" t="s">
         <v>23</v>
       </c>
@@ -1361,8 +1427,8 @@
       <c r="A17" s="3">
         <v>13</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="38"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="35"/>
       <c r="D17" s="7" t="s">
         <v>23</v>
       </c>
@@ -1384,8 +1450,8 @@
       <c r="A18" s="3">
         <v>15</v>
       </c>
-      <c r="B18" s="37"/>
-      <c r="C18" s="38"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="35"/>
       <c r="D18" s="7" t="s">
         <v>23</v>
       </c>
@@ -1407,8 +1473,8 @@
       <c r="A19" s="3">
         <v>16</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="38"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="35"/>
       <c r="D19" s="7" t="s">
         <v>23</v>
       </c>
@@ -1426,7 +1492,30 @@
       <c r="J19" s="32"/>
       <c r="K19" s="3"/>
     </row>
-    <row r="20" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:11" ht="96" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>17</v>
+      </c>
+      <c r="B20" s="34"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="11">
+        <v>45518</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H20" s="30"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="3"/>
+    </row>
+    <row r="21" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C5:C6"/>

</xml_diff>

<commit_message>
commit qa 3_1 19/08/2024 by Hieudn
</commit_message>
<xml_diff>
--- a/QA/通訳サービス_QA表_VN.xlsx
+++ b/QA/通訳サービス_QA表_VN.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\zeus-tmp\QA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieudn\Desktop\WorkingSpace\HPO\zeus-tmp\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5A3CD2-B7AF-46DA-BBAD-94C76261369D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9BF91D-FD6D-4E3A-9B22-27703BD48A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QA表" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="68">
   <si>
     <t>No</t>
   </si>
@@ -299,6 +299,15 @@
   </si>
   <si>
     <t>データの検証</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tại mục 3 đến 6 chúng tôi thấy ở mục 3 sẽ sửa giao diện khá nhiều ở trang quản trị, vậy có thể share cho chúng tôi source code được không? </t>
+  </si>
+  <si>
+    <t>Tại mục 3_1, phần api của memo, video download lấy ở đâu? Nếu chưa có thì khi có cuộc gọi đến chúng tôi sẽ lưu lại màn hình call riêng của operator, của riêng khách hàng, hay của cả khách hàng và operator.</t>
+  </si>
+  <si>
+    <t>tại mục 3_1theo bản dịch thì tôi đang thấy ở mục 16 là confirm video vậy tức là cơ chế của button 17 và 27 giống nhau đúng không? Nếu khác thì button 17 download data gì?</t>
   </si>
 </sst>
 </file>
@@ -416,7 +425,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -566,12 +575,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -677,6 +725,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -992,13 +1057,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:K21"/>
+  <dimension ref="A2:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="H20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
+      <selection pane="bottomRight" activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1446,7 +1511,7 @@
       <c r="J17" s="32"/>
       <c r="K17" s="3"/>
     </row>
-    <row r="18" spans="1:11" ht="42" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="55.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>15</v>
       </c>
@@ -1492,7 +1557,7 @@
       <c r="J19" s="32"/>
       <c r="K19" s="3"/>
     </row>
-    <row r="20" spans="1:11" ht="96" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="95.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>17</v>
       </c>
@@ -1510,12 +1575,93 @@
       <c r="G20" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H20" s="30"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="3"/>
-    </row>
-    <row r="21" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="43"/>
+    </row>
+    <row r="21" spans="1:11" ht="27" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>18</v>
+      </c>
+      <c r="B21" s="34"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="11">
+        <v>45523</v>
+      </c>
+      <c r="G21" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="H21" s="44"/>
+      <c r="I21" s="45"/>
+      <c r="J21" s="45"/>
+      <c r="K21" s="45"/>
+    </row>
+    <row r="22" spans="1:11" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>19</v>
+      </c>
+      <c r="B22" s="34"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="11">
+        <v>45523</v>
+      </c>
+      <c r="G22" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="H22" s="44"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="45"/>
+    </row>
+    <row r="23" spans="1:11" ht="27" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>20</v>
+      </c>
+      <c r="B23" s="34"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F23" s="11">
+        <v>45523</v>
+      </c>
+      <c r="G23" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="H23" s="44"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="45"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="45"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C5:C6"/>

</xml_diff>

<commit_message>
add qa by HieuDN 20/08/2024
</commit_message>
<xml_diff>
--- a/QA/通訳サービス_QA表_VN.xlsx
+++ b/QA/通訳サービス_QA表_VN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hieudn\Desktop\WorkingSpace\HPO\zeus-tmp\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9BF91D-FD6D-4E3A-9B22-27703BD48A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E909BE60-E4F1-42E0-8D41-2E78AEB03ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="74">
   <si>
     <t>No</t>
   </si>
@@ -301,13 +301,31 @@
     <t>データの検証</t>
   </si>
   <si>
-    <t xml:space="preserve">Tại mục 3 đến 6 chúng tôi thấy ở mục 3 sẽ sửa giao diện khá nhiều ở trang quản trị, vậy có thể share cho chúng tôi source code được không? </t>
-  </si>
-  <si>
     <t>Tại mục 3_1, phần api của memo, video download lấy ở đâu? Nếu chưa có thì khi có cuộc gọi đến chúng tôi sẽ lưu lại màn hình call riêng của operator, của riêng khách hàng, hay của cả khách hàng và operator.</t>
   </si>
   <si>
     <t>tại mục 3_1theo bản dịch thì tôi đang thấy ở mục 16 là confirm video vậy tức là cơ chế của button 17 và 27 giống nhau đúng không? Nếu khác thì button 17 download data gì?</t>
+  </si>
+  <si>
+    <t>Phần category bổ xung ở 3-1 và 4-1 pulldown đã có label nhưng phần value truyền vào là dạng nào (số hay chữ theo label)? Cụ thể cho từng mục trong category?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ở phần 5-1 Operator gọi khách hàng, nếu như khách hàng không phản hồi thì tối đa bao nhiêu giây để tự động kết thúc cuộc gọi và phần message thông báo với Operator sẽ như thế nào? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ở phần 5-1và 3-1 ô nhập customer ID sẽ validate như nào? Bao nhiêu kí tự, viết hoa viết thường gì không? </t>
+  </si>
+  <si>
+    <t>Ở mục 4-1, phản ánh tự động sẽ lấy ở đâu? Đã có api chưa? Nếu chưa có thì chúng tôi phải xây dựng api mới và cơ chế tính toán của phản ánh tự động như nào?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tại mục 3 đến 5 chúng tôi thấy ở mục 3 sẽ sửa giao diện khá nhiều ở trang quản trị, vậy có thể share cho chúng tôi source code được không? </t>
+  </si>
+  <si>
+    <t>Ở phần 5-1 Operator gọi khách hàng, việc xây dựng api video call sẽ sử dụng công nghệ gì để xử lí video call amazon chime sdk hay webrtc? Có lưu trữ lại các file video tại s3 hay nơi nào đó không?</t>
+  </si>
+  <si>
+    <t>Ở phần 5-1 Operator gọi khách hàng, có button confirm, chúng tôi đang hiểu là khi nhập ID customer sau đó nút confirm để xác nhận ID customer tồn tại? Vậy việc query sẽ như thế nào? Trường dữ liệu tên gì? Table nào? Dữ liệu query ở đâu?</t>
   </si>
 </sst>
 </file>
@@ -317,7 +335,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -404,8 +422,14 @@
       <name val="MS PGothic"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="MS PGothic"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -421,6 +445,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -619,7 +649,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -716,15 +746,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -742,6 +763,39 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1057,13 +1111,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:K24"/>
+  <dimension ref="A2:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="H20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="H29" sqref="H29"/>
+      <selection pane="bottomRight" activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,7 +1185,7 @@
       <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="43" t="s">
         <v>39</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -1162,7 +1216,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="9"/>
-      <c r="C6" s="37"/>
+      <c r="C6" s="44"/>
       <c r="D6" s="7" t="s">
         <v>16</v>
       </c>
@@ -1193,7 +1247,7 @@
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="43" t="s">
         <v>40</v>
       </c>
       <c r="D7" s="7" t="s">
@@ -1224,7 +1278,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="10"/>
-      <c r="C8" s="38"/>
+      <c r="C8" s="45"/>
       <c r="D8" s="7" t="s">
         <v>17</v>
       </c>
@@ -1253,7 +1307,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="10"/>
-      <c r="C9" s="38"/>
+      <c r="C9" s="45"/>
       <c r="D9" s="7" t="s">
         <v>18</v>
       </c>
@@ -1282,7 +1336,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="10"/>
-      <c r="C10" s="37"/>
+      <c r="C10" s="44"/>
       <c r="D10" s="7" t="s">
         <v>19</v>
       </c>
@@ -1311,7 +1365,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="10"/>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="43" t="s">
         <v>41</v>
       </c>
       <c r="D11" s="7" t="s">
@@ -1342,7 +1396,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="9"/>
-      <c r="C12" s="37"/>
+      <c r="C12" s="44"/>
       <c r="D12" s="7" t="s">
         <v>21</v>
       </c>
@@ -1373,7 +1427,7 @@
       <c r="B13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="43" t="s">
         <v>42</v>
       </c>
       <c r="D13" s="7" t="s">
@@ -1404,7 +1458,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="9"/>
-      <c r="C14" s="37"/>
+      <c r="C14" s="44"/>
       <c r="D14" s="7" t="s">
         <v>22</v>
       </c>
@@ -1575,10 +1629,10 @@
       <c r="G20" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H20" s="40"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="43"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="40"/>
     </row>
     <row r="21" spans="1:11" ht="27" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
@@ -1586,22 +1640,20 @@
       </c>
       <c r="B21" s="34"/>
       <c r="C21" s="35"/>
-      <c r="D21" s="7" t="s">
-        <v>23</v>
-      </c>
+      <c r="D21" s="7"/>
       <c r="E21" s="8" t="s">
         <v>58</v>
       </c>
       <c r="F21" s="11">
         <v>45523</v>
       </c>
-      <c r="G21" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="H21" s="44"/>
-      <c r="I21" s="45"/>
-      <c r="J21" s="45"/>
-      <c r="K21" s="45"/>
+      <c r="G21" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="H21" s="41"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="42"/>
     </row>
     <row r="22" spans="1:11" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
@@ -1609,22 +1661,20 @@
       </c>
       <c r="B22" s="34"/>
       <c r="C22" s="35"/>
-      <c r="D22" s="7" t="s">
-        <v>23</v>
-      </c>
+      <c r="D22" s="7"/>
       <c r="E22" s="8" t="s">
         <v>58</v>
       </c>
       <c r="F22" s="11">
         <v>45523</v>
       </c>
-      <c r="G22" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="H22" s="44"/>
-      <c r="I22" s="45"/>
-      <c r="J22" s="45"/>
-      <c r="K22" s="45"/>
+      <c r="G22" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="H22" s="41"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="42"/>
     </row>
     <row r="23" spans="1:11" ht="27" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
@@ -1632,35 +1682,149 @@
       </c>
       <c r="B23" s="34"/>
       <c r="C23" s="35"/>
-      <c r="D23" s="7" t="s">
-        <v>23</v>
-      </c>
+      <c r="D23" s="7"/>
       <c r="E23" s="8" t="s">
         <v>58</v>
       </c>
       <c r="F23" s="11">
         <v>45523</v>
       </c>
-      <c r="G23" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="H23" s="44"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="45"/>
-      <c r="K23" s="45"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
+      <c r="G23" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="H23" s="41"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="42"/>
+    </row>
+    <row r="24" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>21</v>
+      </c>
       <c r="B24" s="34"/>
       <c r="C24" s="35"/>
       <c r="D24" s="7"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="44"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="45"/>
-      <c r="K24" s="45"/>
+      <c r="E24" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" s="11">
+        <v>45524</v>
+      </c>
+      <c r="G24" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="H24" s="41"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="42"/>
+    </row>
+    <row r="25" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>22</v>
+      </c>
+      <c r="B25" s="34"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" s="11">
+        <v>45524</v>
+      </c>
+      <c r="G25" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="H25" s="41"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="42"/>
+      <c r="K25" s="42"/>
+    </row>
+    <row r="26" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>23</v>
+      </c>
+      <c r="B26" s="34"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F26" s="11">
+        <v>45524</v>
+      </c>
+      <c r="G26" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="H26" s="41"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="42"/>
+      <c r="K26" s="42"/>
+    </row>
+    <row r="27" spans="1:11" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>24</v>
+      </c>
+      <c r="B27" s="34"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" s="11">
+        <v>45524</v>
+      </c>
+      <c r="G27" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="H27" s="41"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
+      <c r="K27" s="42"/>
+    </row>
+    <row r="28" spans="1:11" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="46">
+        <v>25</v>
+      </c>
+      <c r="B28" s="55"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="48"/>
+      <c r="E28" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" s="50">
+        <v>45524</v>
+      </c>
+      <c r="G28" s="51" t="s">
+        <v>73</v>
+      </c>
+      <c r="H28" s="52"/>
+      <c r="I28" s="53"/>
+      <c r="J28" s="53"/>
+      <c r="K28" s="53"/>
+    </row>
+    <row r="29" spans="1:11" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="46">
+        <v>25</v>
+      </c>
+      <c r="B29" s="53"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="48"/>
+      <c r="E29" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="F29" s="50">
+        <v>45524</v>
+      </c>
+      <c r="G29" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="H29" s="52"/>
+      <c r="I29" s="53"/>
+      <c r="J29" s="53"/>
+      <c r="K29" s="53"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H30" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>